<commit_message>
corrected logic for healthscore calculation
</commit_message>
<xml_diff>
--- a/outputs/healthscore_calculado.xlsx
+++ b/outputs/healthscore_calculado.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -793,7 +793,7 @@
         <v>-1</v>
       </c>
       <c r="K7" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8">

</xml_diff>

<commit_message>
Restructures the project - added utils and renamed files. United them at main.py
</commit_message>
<xml_diff>
--- a/outputs/healthscore_calculado.xlsx
+++ b/outputs/healthscore_calculado.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -16,7 +16,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
+  </numFmts>
   <fonts count="2">
     <font>
       <name val="Calibri"/>
@@ -55,11 +58,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -425,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K10"/>
+  <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -456,35 +460,30 @@
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>tags</t>
+          <t>ocorridos</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>ocorridos</t>
+          <t>data</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>data</t>
+          <t>cliente</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>cliente</t>
+          <t>Ranking_de_Eventos</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>Ranking_de_Eventos</t>
+          <t>Delta</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>Delta</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>Healthscore</t>
         </is>
@@ -511,33 +510,26 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>[]</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
           <t>Cliente pediu proposta</t>
         </is>
       </c>
+      <c r="F2" s="2" t="n">
+        <v>45488</v>
+      </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>2024-07-15</t>
+          <t>Cocamar</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Cocamar</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
           <t>Cliente pediu proposta</t>
         </is>
       </c>
+      <c r="I2" t="n">
+        <v>2.5</v>
+      </c>
       <c r="J2" t="n">
-        <v>2.5</v>
-      </c>
-      <c r="K2" t="n">
         <v>10</v>
       </c>
     </row>
@@ -562,33 +554,26 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>[]</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
           <t>Resolveu problema</t>
         </is>
       </c>
+      <c r="F3" s="2" t="n">
+        <v>45488</v>
+      </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>2024-07-15</t>
+          <t>Cocamar</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>Cocamar</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
           <t>Resolveu problema</t>
         </is>
       </c>
+      <c r="I3" t="n">
+        <v>2</v>
+      </c>
       <c r="J3" t="n">
-        <v>2</v>
-      </c>
-      <c r="K3" t="n">
         <v>10</v>
       </c>
     </row>
@@ -613,33 +598,26 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>[]</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
           <t>Metas não atingidas</t>
         </is>
       </c>
+      <c r="F4" s="2" t="n">
+        <v>45488</v>
+      </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>2024-07-15</t>
+          <t>Mart Minas</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>Mart Minas</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
           <t>Metas não atingidas</t>
         </is>
       </c>
+      <c r="I4" t="n">
+        <v>-2</v>
+      </c>
       <c r="J4" t="n">
-        <v>-2</v>
-      </c>
-      <c r="K4" t="n">
         <v>8</v>
       </c>
     </row>
@@ -664,33 +642,26 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>[]</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
           <t>Feedback positivo</t>
         </is>
       </c>
+      <c r="F5" s="2" t="n">
+        <v>45488</v>
+      </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>2024-07-15</t>
+          <t>Mart Minas</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>Mart Minas</t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
           <t>Feedback positivo</t>
         </is>
       </c>
+      <c r="I5" t="n">
+        <v>2.5</v>
+      </c>
       <c r="J5" t="n">
-        <v>2.5</v>
-      </c>
-      <c r="K5" t="n">
         <v>10</v>
       </c>
     </row>
@@ -715,43 +686,36 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>[]</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
           <t>Planejamento foi reprovado</t>
         </is>
       </c>
+      <c r="F6" s="2" t="n">
+        <v>45502</v>
+      </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>2024-07-29</t>
+          <t>FBMDS</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>FBMDS</t>
-        </is>
-      </c>
-      <c r="I6" t="inlineStr">
-        <is>
           <t>Planejamento foi reprovado</t>
         </is>
       </c>
+      <c r="I6" t="n">
+        <v>-1</v>
+      </c>
       <c r="J6" t="n">
-        <v>-1</v>
-      </c>
-      <c r="K6" t="n">
         <v>9</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>156244</v>
+        <v>156243</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>FBMDS, 29/07/2024</t>
+          <t>Litero, 05/08/2024</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -766,34 +730,27 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>[]</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>Houve atraso nas entregas, isso prejudicou os clientes</t>
-        </is>
+          <t>Cliente pediu proposta</t>
+        </is>
+      </c>
+      <c r="F7" s="2" t="n">
+        <v>45509</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>2024-07-29</t>
+          <t>Litero</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>FBMDS</t>
-        </is>
-      </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>Houve atraso nas entregas, isso prejudicou os clientes</t>
-        </is>
+          <t>Cliente pediu proposta</t>
+        </is>
+      </c>
+      <c r="I7" t="n">
+        <v>2.5</v>
       </c>
       <c r="J7" t="n">
-        <v>-1</v>
-      </c>
-      <c r="K7" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8">
@@ -817,43 +774,36 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>[]</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>Cliente pediu proposta</t>
-        </is>
+          <t>Feedback positivo</t>
+        </is>
+      </c>
+      <c r="F8" s="2" t="n">
+        <v>45509</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>2024-08-05</t>
+          <t>Litero</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>Litero</t>
-        </is>
-      </c>
-      <c r="I8" t="inlineStr">
-        <is>
-          <t>Cliente pediu proposta</t>
-        </is>
+          <t>Feedback positivo</t>
+        </is>
+      </c>
+      <c r="I8" t="n">
+        <v>2.5</v>
       </c>
       <c r="J8" t="n">
-        <v>2.5</v>
-      </c>
-      <c r="K8" t="n">
         <v>10</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>156243</v>
+        <v>160421</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Litero, 05/08/2024</t>
+          <t>Cliente_fake, 19/08/2024</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -868,43 +818,32 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>[]</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>Feedback positivo</t>
-        </is>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>2024-08-05</t>
-        </is>
-      </c>
+          <t>Feedback negativo</t>
+        </is>
+      </c>
+      <c r="F9" s="2" t="n">
+        <v>45523</v>
+      </c>
+      <c r="G9" t="inlineStr"/>
       <c r="H9" t="inlineStr">
         <is>
-          <t>Litero</t>
-        </is>
-      </c>
-      <c r="I9" t="inlineStr">
-        <is>
-          <t>Feedback positivo</t>
-        </is>
+          <t>Feedback negativo</t>
+        </is>
+      </c>
+      <c r="I9" t="n">
+        <v>-2.5</v>
       </c>
       <c r="J9" t="n">
-        <v>2.5</v>
-      </c>
-      <c r="K9" t="n">
-        <v>10</v>
+        <v>7.5</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>154950</v>
+        <v>160421</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Mart Minas, 12/08/2024</t>
+          <t>Cliente_fake, 19/08/2024</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -919,34 +858,151 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>[]</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>Houve atraso nas entregas, isso prejudicou os clientes</t>
-        </is>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>2024-08-12</t>
-        </is>
-      </c>
+          <t>Cliente não responde (NPS ou outra comunicação) | No-show</t>
+        </is>
+      </c>
+      <c r="F10" s="2" t="n">
+        <v>45523</v>
+      </c>
+      <c r="G10" t="inlineStr"/>
       <c r="H10" t="inlineStr">
         <is>
+          <t>Cliente não responde (NPS ou outra comunicação) | No-show</t>
+        </is>
+      </c>
+      <c r="I10" t="n">
+        <v>-2</v>
+      </c>
+      <c r="J10" t="n">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>160421</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Cliente_fake, 19/08/2024</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>backlog</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Acompanhamento de clientes</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Planejamento foi reprovado</t>
+        </is>
+      </c>
+      <c r="F11" s="2" t="n">
+        <v>45523</v>
+      </c>
+      <c r="G11" t="inlineStr"/>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>Planejamento foi reprovado</t>
+        </is>
+      </c>
+      <c r="I11" t="n">
+        <v>-1</v>
+      </c>
+      <c r="J11" t="n">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>160794</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Mart Minas, 26/08/2024</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>backlog</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Acompanhamento de clientes</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>Planejamento foi reprovado</t>
+        </is>
+      </c>
+      <c r="F12" s="2" t="n">
+        <v>45530</v>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
           <t>Mart Minas</t>
         </is>
       </c>
-      <c r="I10" t="inlineStr">
-        <is>
-          <t>Houve atraso nas entregas, isso prejudicou os clientes</t>
-        </is>
-      </c>
-      <c r="J10" t="n">
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>Planejamento foi reprovado</t>
+        </is>
+      </c>
+      <c r="I12" t="n">
         <v>-1</v>
       </c>
-      <c r="K10" t="n">
+      <c r="J12" t="n">
         <v>9</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>165463</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Mart Minas, 09/09/2024</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>backlog</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Acompanhamento de clientes</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Feedback negativo</t>
+        </is>
+      </c>
+      <c r="F13" s="2" t="n">
+        <v>45544</v>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>Mart Minas</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>Feedback negativo</t>
+        </is>
+      </c>
+      <c r="I13" t="n">
+        <v>-2.5</v>
+      </c>
+      <c r="J13" t="n">
+        <v>6.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>